<commit_message>
Data have img info
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AEA345-CB62-4F6A-9DCD-AE5BE261E9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A15CE4-7331-4C72-84BD-25D6F512EA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-28800" yWindow="4695" windowWidth="25830" windowHeight="11625" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,6 +70,43 @@
   </si>
   <si>
     <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imgsrc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pivot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5,0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5,0.1875</t>
+  </si>
+  <si>
+    <t>0.5,0.1875</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Tower/1001.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Tower/1002.png</t>
+  </si>
+  <si>
+    <t>/Enemy/2001.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Enemy/2002.png</t>
+  </si>
+  <si>
+    <t>pixelperunit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -116,9 +153,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,134 +478,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53B544D-229D-4A5B-BFF8-79DA3F65400C}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="18.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.25" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2001</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>5</v>
+      <c r="E2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2002</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>5</v>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{03BE8DB2-3E4C-4C0E-9BF1-528DB96C6C60}">
+      <formula1>COUNTIFS($A:$A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B29847-794D-4111-A9E5-2858606572C7}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="18.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.25" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>5</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{1F15BD78-2C76-416A-AA9B-FA64F5D504AF}">
+      <formula1>COUNTIF(A:A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enemy Dark Elf Design
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D269137-645B-4C80-925D-D945FE54A38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760FBB43-4F0F-49F7-B5B2-A9B1126246EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21225" yWindow="6600" windowWidth="19425" windowHeight="12165" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="EnumData" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,6 +303,14 @@
   </si>
   <si>
     <t>3,3,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020100,2020101,2020102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021103,2021104,2022105</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -902,7 +910,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -936,7 +944,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>44</v>
@@ -944,10 +952,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Description popup with ID
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3002EA-EC6A-445C-BFBE-7D2570DDC2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F681C37D-1C2D-4BC1-B140-342927ADAE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="13500" windowWidth="19425" windowHeight="12165" firstSheet="3" activeTab="6" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-20100" yWindow="5265" windowWidth="18075" windowHeight="14130" firstSheet="3" activeTab="7" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWER@FIRE" sheetId="9" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="ENEMY@WATER" sheetId="13" r:id="rId5"/>
     <sheet name="ENEMY@NATURE" sheetId="14" r:id="rId6"/>
     <sheet name="STAT" sheetId="15" r:id="rId7"/>
-    <sheet name="EnumData" sheetId="7" r:id="rId8"/>
-    <sheet name="Round" sheetId="8" r:id="rId9"/>
+    <sheet name="UI" sheetId="16" r:id="rId8"/>
+    <sheet name="EnumData" sheetId="7" r:id="rId9"/>
+    <sheet name="Round" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="200">
   <si>
     <t>POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2312,6 +2313,86 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3433CC4-0965-4602-82C6-05F8C3A6D438}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A7" xr:uid="{F85E7059-D32B-4D8F-97DE-23444DAF66C9}">
+      <formula1>COUNTIFS($A:$A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3F0F3C-A656-4EC0-A859-21F1263F0A34}">
   <dimension ref="A1:S36"/>
@@ -5386,8 +5467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF271AF4-E94B-43D7-A6A9-013F378630A5}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5718,6 +5799,35 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8E4527-3365-487A-B440-8E1995F53AC4}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{41BF5432-82E9-4C52-9DEB-55ECF7CE15FC}">
+      <formula1>COUNTIF(A:A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E51131-8292-4C96-A8C6-57F82B798DDF}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -5941,84 +6051,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3433CC4-0965-4602-82C6-05F8C3A6D438}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A7" xr:uid="{F85E7059-D32B-4D8F-97DE-23444DAF66C9}">
-      <formula1>COUNTIFS($A:$A,A1)=1</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Enemy Design by Element
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A92DD43-5C40-4BEB-9DFE-E646C8103267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6528E72E-21A6-4521-B69A-8EDAD6B4FCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20100" yWindow="5265" windowWidth="18075" windowHeight="14130" firstSheet="3" activeTab="8" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-20100" yWindow="5265" windowWidth="18075" windowHeight="14130" firstSheet="3" activeTab="3" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWER@FIRE" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="240">
   <si>
     <t>POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -635,10 +635,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>다크엘프,Dark Elf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>오크,Orc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -896,6 +892,110 @@
   </si>
   <si>
     <t>EnemyGrade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 오크,Ice Orc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 오크병사,Ice Orc Solider</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 오크도끼전사,Ice Orc Axe Soldier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정예 아이스 오크도끼전사, Elite Ice Orc Axe Solider</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자이언트 아이스 오크, Giant Ice Orc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 오크샤먼, Shaman Ice Orc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 다크엘프 검사,Ice Dark Elf Soldier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 다크엘프 창술사,Ice Dark Elf Spearman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 다크엘프 어쌔신,Ice Dark Elf Assassin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 다크엘프 마법사,Ice Dark Elf Mage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 다크엘프 마검사,Ice Dark Elf Magic Knight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 다크엘프 로드,Ice Dark Elf Lord</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 오크,Fire Orc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 오크병사,Fire Orc Solider</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 오크도끼전사,Fire Orc Axe Soldier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정예 파이어 오크도끼전사, Elite Fire Orc Axe Solider</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자이언트 파이어 오크, Giant Fire Orc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 오크샤먼, Shaman Fire Orc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 오크 족장, Chief Fire Orc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 오크 족장, Chief Ice Orc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 다크엘프 검사,Fire Dark Elf Soldier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 다크엘프 창술사,Fire Dark Elf Spearman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 다크엘프 어쌔신,Fire Dark Elf Assassin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 다크엘프 마법사,Fire Dark Elf Mage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 다크엘프 마검사,Fire Dark Elf Magic Knight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이어 다크엘프 로드,Fire Dark Elf Lord</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4736,11 +4836,1063 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75967C55-9BA4-40EE-BBD0-AF03F89CCB6F}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f t="shared" ref="I2:I15" si="0">CONCATENATE("/Sprites/Enemy/",A2,"/")</f>
+        <v>/Sprites/Enemy/2000000/</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2000001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2000001/</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2000002</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2000002/</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>2001002</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2001002/</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2001003</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2001003/</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>2001004</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2001004/</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2002005</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>50</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2002005/</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2000100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>50</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2000100/</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2000101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>50</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2000101/</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>2000102</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2000102/</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>2001102</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>50</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2001102/</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>2001103</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>50</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2001103/</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>2001104</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>50</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2001104/</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2002105</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>50</v>
+      </c>
+      <c r="H15" s="1">
+        <v>5</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2002105/</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{1F15BD78-2C76-416A-AA9B-FA64F5D504AF}">
+      <formula1>COUNTIF(A:A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C28BD20-4060-4017-8FFF-9C9E3C00F1E8}">
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>2010000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f t="shared" ref="I2:I15" si="0">CONCATENATE("/Sprites/Enemy/",A2,"/")</f>
+        <v>/Sprites/Enemy/2010000/</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2010001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2010001/</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2010002</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2010002/</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>2011002</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2011002/</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2011003</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2011003/</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>2011004</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2011004/</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2012005</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>50</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2012005/</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2010100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>50</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2010100/</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2010101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>50</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2010101/</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>2010102</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2010102/</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>2011102</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>50</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2011102/</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>2011103</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>50</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2011103/</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>2011104</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>50</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2011104/</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2012105</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>50</v>
+      </c>
+      <c r="H15" s="1">
+        <v>5</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/2012105/</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{C599AA2A-F464-4210-92BD-79E3075BDA2F}">
+      <formula1>COUNTIF(A:A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F511731-D966-487D-B559-FFB18F3F2C14}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="A2:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4761,286 +5913,22 @@
         <v>111</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>109</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>2000000</v>
-      </c>
-      <c r="B2" t="s">
         <v>150</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>50</v>
-      </c>
-      <c r="H2" s="1">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f>CONCATENATE("/Sprites/Enemy/",A2,"/")</f>
-        <v>/Sprites/Enemy/2000000/</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2000100</v>
-      </c>
-      <c r="B3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>50</v>
-      </c>
-      <c r="H3" s="1">
-        <v>5</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <f>CONCATENATE("/Sprites/Enemy/",A3,"/")</f>
-        <v>/Sprites/Enemy/2000100/</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{1F15BD78-2C76-416A-AA9B-FA64F5D504AF}">
-      <formula1>COUNTIF(A:A,A1)=1</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C28BD20-4060-4017-8FFF-9C9E3C00F1E8}">
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>2010000</v>
-      </c>
-      <c r="B2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>50</v>
-      </c>
-      <c r="H2" s="1">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f>CONCATENATE("/Sprites/Enemy/",A2,"/")</f>
-        <v>/Sprites/Enemy/2010000/</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2010100</v>
-      </c>
-      <c r="B3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>50</v>
-      </c>
-      <c r="H3" s="1">
-        <v>5</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <f>CONCATENATE("/Sprites/Enemy/",A3,"/")</f>
-        <v>/Sprites/Enemy/2010100/</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B4"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576 A1:A2" xr:uid="{C599AA2A-F464-4210-92BD-79E3075BDA2F}">
-      <formula1>COUNTIF(A:A,A1)=1</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F511731-D966-487D-B559-FFB18F3F2C14}">
-  <dimension ref="A1:K15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>95</v>
@@ -5055,7 +5943,7 @@
         <v>2020000</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -5088,7 +5976,7 @@
         <v>2020001</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -5121,7 +6009,7 @@
         <v>2020002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -5154,7 +6042,7 @@
         <v>2021002</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -5187,7 +6075,7 @@
         <v>2021003</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -5220,7 +6108,7 @@
         <v>2021004</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -5253,7 +6141,7 @@
         <v>2022005</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -5286,7 +6174,7 @@
         <v>2020100</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -5319,7 +6207,7 @@
         <v>2020101</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -5352,7 +6240,7 @@
         <v>2020102</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -5385,7 +6273,7 @@
         <v>2021102</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -5418,7 +6306,7 @@
         <v>2021103</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -5451,7 +6339,7 @@
         <v>2021104</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -5484,7 +6372,7 @@
         <v>2022105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -5550,7 +6438,7 @@
         <v>3000000</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5558,7 +6446,7 @@
         <v>3000001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5570,7 +6458,7 @@
         <v>3001999</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5578,7 +6466,7 @@
         <v>3001000</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5586,7 +6474,7 @@
         <v>3001001</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5594,7 +6482,7 @@
         <v>3001002</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5605,7 +6493,7 @@
         <v>3002000</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5613,7 +6501,7 @@
         <v>3002001</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -5621,7 +6509,7 @@
         <v>3002002</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -5629,7 +6517,7 @@
         <v>3002003</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -5637,7 +6525,7 @@
         <v>3003000</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -5645,7 +6533,7 @@
         <v>3003001</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -5653,7 +6541,7 @@
         <v>3003002</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -5669,7 +6557,7 @@
         <v>3004001</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -5677,7 +6565,7 @@
         <v>3004002</v>
       </c>
       <c r="B21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -5685,7 +6573,7 @@
         <v>3004003</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -5693,7 +6581,7 @@
         <v>3100000</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -5701,7 +6589,7 @@
         <v>3100001</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -5709,7 +6597,7 @@
         <v>3100002</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -5717,7 +6605,7 @@
         <v>3100003</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -5725,7 +6613,7 @@
         <v>3101000</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -5733,7 +6621,7 @@
         <v>3101001</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -5741,7 +6629,7 @@
         <v>3101002</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -5749,7 +6637,7 @@
         <v>3101003</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -5757,7 +6645,7 @@
         <v>3101004</v>
       </c>
       <c r="B33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -5765,7 +6653,7 @@
         <v>3101005</v>
       </c>
       <c r="B34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -5773,7 +6661,7 @@
         <v>3200000</v>
       </c>
       <c r="B36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -5781,7 +6669,7 @@
         <v>3200001</v>
       </c>
       <c r="B37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -5789,7 +6677,7 @@
         <v>3200002</v>
       </c>
       <c r="B38" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -5797,7 +6685,7 @@
         <v>3200003</v>
       </c>
       <c r="B39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -5805,7 +6693,7 @@
         <v>3200004</v>
       </c>
       <c r="B40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -5813,7 +6701,7 @@
         <v>3201000</v>
       </c>
       <c r="B42" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -5821,7 +6709,7 @@
         <v>3201001</v>
       </c>
       <c r="B43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -5829,7 +6717,7 @@
         <v>3201002</v>
       </c>
       <c r="B44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -5837,7 +6725,7 @@
         <v>3201003</v>
       </c>
       <c r="B45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -5845,7 +6733,7 @@
         <v>3201004</v>
       </c>
       <c r="B46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -5853,7 +6741,7 @@
         <v>3201005</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -5861,7 +6749,7 @@
         <v>3300000</v>
       </c>
       <c r="B49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -5869,7 +6757,7 @@
         <v>3300001</v>
       </c>
       <c r="B50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -5877,7 +6765,7 @@
         <v>3300002</v>
       </c>
       <c r="B51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -5885,7 +6773,7 @@
         <v>3301000</v>
       </c>
       <c r="B53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -5893,7 +6781,7 @@
         <v>3301001</v>
       </c>
       <c r="B54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -5901,7 +6789,7 @@
         <v>3301002</v>
       </c>
       <c r="B55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -5948,7 +6836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E51131-8292-4C96-A8C6-57F82B798DDF}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -6013,16 +6901,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" t="s">
         <v>211</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>212</v>
-      </c>
-      <c r="D4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -6067,16 +6955,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" t="s">
         <v>201</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>202</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>203</v>
-      </c>
-      <c r="D7" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Unit Editor Edit Unit
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6528E72E-21A6-4521-B69A-8EDAD6B4FCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3A8E76-3863-44A2-AC6E-88E20F2E0127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20100" yWindow="5265" windowWidth="18075" windowHeight="14130" firstSheet="3" activeTab="3" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-20370" yWindow="5655" windowWidth="18075" windowHeight="14130" firstSheet="4" activeTab="7" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWER@FIRE" sheetId="9" r:id="rId1"/>
     <sheet name="TOWER@WATER" sheetId="10" r:id="rId2"/>
     <sheet name="TOWER@NATURE" sheetId="11" r:id="rId3"/>
-    <sheet name="ENEMY@FIRE" sheetId="12" r:id="rId4"/>
-    <sheet name="ENEMY@WATER" sheetId="13" r:id="rId5"/>
-    <sheet name="ENEMY@NATURE" sheetId="14" r:id="rId6"/>
-    <sheet name="STAT" sheetId="15" r:id="rId7"/>
-    <sheet name="UI" sheetId="16" r:id="rId8"/>
-    <sheet name="EnumData" sheetId="7" r:id="rId9"/>
-    <sheet name="Round" sheetId="8" r:id="rId10"/>
+    <sheet name="TOWER@CUSTOM" sheetId="17" r:id="rId4"/>
+    <sheet name="ENEMY@FIRE" sheetId="12" r:id="rId5"/>
+    <sheet name="ENEMY@WATER" sheetId="13" r:id="rId6"/>
+    <sheet name="ENEMY@NATURE" sheetId="14" r:id="rId7"/>
+    <sheet name="ENEMY@CUSTOM" sheetId="18" r:id="rId8"/>
+    <sheet name="STAT" sheetId="15" r:id="rId9"/>
+    <sheet name="UI" sheetId="16" r:id="rId10"/>
+    <sheet name="EnumData" sheetId="7" r:id="rId11"/>
+    <sheet name="Round" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="240">
   <si>
     <t>POWER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1374,14 +1376,15 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U10" sqref="U10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="6" width="9" style="1"/>
     <col min="9" max="9" width="9" style="1"/>
-    <col min="10" max="12" width="9" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
     <col min="14" max="14" width="9" style="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="1"/>
@@ -2474,6 +2477,289 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8E4527-3365-487A-B440-8E1995F53AC4}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{41BF5432-82E9-4C52-9DEB-55ECF7CE15FC}">
+      <formula1>COUNTIF(A:A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E51131-8292-4C96-A8C6-57F82B798DDF}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3433CC4-0965-4602-82C6-05F8C3A6D438}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2557,9 +2843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3F0F3C-A656-4EC0-A859-21F1263F0A34}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1:T23"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3665,7 +3951,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4835,12 +5121,724 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5381F8-97C8-4316-9E8C-10D9ECA24755}">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="9" style="1"/>
+    <col min="9" max="9" width="9" style="1"/>
+    <col min="10" max="11" width="9" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="1"/>
+    <col min="14" max="14" width="9" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="1"/>
+    <col min="18" max="18" width="25" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>4000000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="1">
+        <v>150</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R2" s="1" t="str">
+        <f t="shared" ref="R2:R14" si="0">CONCATENATE("/Sprites/Tower/",A2,"/")</f>
+        <v>/Sprites/Tower/4000000/</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>4000001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="1">
+        <v>150</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="R3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Tower/4000001/</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>4000002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="1">
+        <v>150</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>147</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Tower/4000002/</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4000003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="1">
+        <v>150</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Tower/4000003/</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4010000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="1">
+        <v>150</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Tower/4010000/</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>4010001</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="1">
+        <v>150</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <f>CONCATENATE("/Sprites/Tower/",A7,"/")</f>
+        <v>/Sprites/Tower/4010001/</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>4011001</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="1">
+        <v>150</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <f>CONCATENATE("/Sprites/Tower/",A8,"/")</f>
+        <v>/Sprites/Tower/4011001/</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>4012001</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="1">
+        <v>150</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="R9" s="1" t="str">
+        <f>CONCATENATE("/Sprites/Tower/",A9,"/")</f>
+        <v>/Sprites/Tower/4012001/</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>4010002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="1">
+        <v>150</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="N10" t="s">
+        <v>116</v>
+      </c>
+      <c r="O10"/>
+      <c r="R10" s="1" t="str">
+        <f t="shared" ref="R10" si="1">CONCATENATE("/Sprites/Tower/",A10,"/")</f>
+        <v>/Sprites/Tower/4010002/</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>4020000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="1">
+        <v>150</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="R11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Tower/4020000/</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>4020001</v>
+      </c>
+      <c r="B12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="1">
+        <v>150</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Tower/4020001/</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>4020002</v>
+      </c>
+      <c r="B13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="1">
+        <v>150</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="R13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Tower/4020002/</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>4020005</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="1">
+        <v>150</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="R14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Tower/4020005/</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B15"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27:A1048576 A1:A25" xr:uid="{AB708ADF-5841-4EF2-8D25-37A7A73C0567}">
+      <formula1>COUNTIFS($A:$A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75967C55-9BA4-40EE-BBD0-AF03F89CCB6F}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5115,7 +6113,7 @@
         <v>/Sprites/Enemy/2002005/</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -5360,13 +6358,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C28BD20-4060-4017-8FFF-9C9E3C00F1E8}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5641,7 +6639,7 @@
         <v>/Sprites/Enemy/2012005/</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -5886,13 +6884,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F511731-D966-487D-B559-FFB18F3F2C14}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="A2:J15"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6166,7 +7164,7 @@
         <v>/Sprites/Enemy/2022005/</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -6411,12 +7409,537 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3772D7-A36A-432F-9AE3-217645637BC6}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>5020000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f t="shared" ref="I2:I15" si="0">CONCATENATE("/Sprites/Enemy/",A2,"/")</f>
+        <v>/Sprites/Enemy/5020000/</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>5020001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5020001/</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>5020002</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5020002/</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>5021002</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5021002/</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5021003</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5021003/</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5021004</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5021004/</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>5022005</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>50</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5022005/</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>5020100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>50</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5020100/</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>5020101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>50</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5020101/</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>5020102</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5020102/</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>5021102</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>50</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5021102/</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>5021103</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>50</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5021103/</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>5021104</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>50</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5021104/</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>5022105</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>50</v>
+      </c>
+      <c r="H15" s="1">
+        <v>5</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>/Sprites/Enemy/5022105/</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{93E42DEC-E91E-4B23-B621-016AD9606CB5}">
+      <formula1>COUNTIF(A:A,A1)=1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF271AF4-E94B-43D7-A6A9-013F378630A5}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6801,287 +8324,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8E4527-3365-487A-B440-8E1995F53AC4}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{41BF5432-82E9-4C52-9DEB-55ECF7CE15FC}">
-      <formula1>COUNTIF(A:A,A1)=1</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E51131-8292-4C96-A8C6-57F82B798DDF}">
-  <dimension ref="A1:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>213</v>
-      </c>
-      <c r="B4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Unit Editor Save Tower
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3A8E76-3863-44A2-AC6E-88E20F2E0127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20233525-CB68-4DC6-9FA4-EFEB8CD02EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20370" yWindow="5655" windowWidth="18075" windowHeight="14130" firstSheet="4" activeTab="7" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-20370" yWindow="5655" windowWidth="18075" windowHeight="14130" firstSheet="6" activeTab="10" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWER@FIRE" sheetId="9" r:id="rId1"/>
@@ -2509,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E51131-8292-4C96-A8C6-57F82B798DDF}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7413,7 +7413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3772D7-A36A-432F-9AE3-217645637BC6}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>

</xml_diff>

<commit_message>
Adjust Tower Activation Mechanism
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76696083-E0DD-4586-A806-B6518C940550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDB3505-CBD5-4DFD-AB66-DC57EE8D67EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27600" yWindow="5355" windowWidth="18075" windowHeight="14130" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-28455" yWindow="5730" windowWidth="18075" windowHeight="14130" tabRatio="831" firstSheet="1" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWER@FIRE" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="245">
   <si>
     <t>ATTACKSPEED</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1012,6 +1012,10 @@
   </si>
   <si>
     <t>1,1.5;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101,1;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1388,7 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F370FB-69E7-436B-99AD-BE543F2F51A7}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
@@ -2569,9 +2573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3F0F3C-A656-4EC0-A859-21F1263F0A34}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1:Q1048576"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2666,6 +2670,9 @@
       <c r="I2" s="1">
         <v>0</v>
       </c>
+      <c r="O2" t="s">
+        <v>244</v>
+      </c>
       <c r="P2" s="1" t="str">
         <f t="shared" ref="P2:P23" si="0">CONCATENATE("/Sprites/Tower/",A2,"/")</f>
         <v>/Sprites/Tower/1010000/</v>
@@ -3670,9 +3677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4F02CE-18E1-4CEC-BC57-9C41A68A4035}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1:Q1048576"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4513,7 +4520,7 @@
         <v>150</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1">
         <v>2.5</v>
@@ -4552,7 +4559,7 @@
         <v>150</v>
       </c>
       <c r="D20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
         <v>2.5</v>
@@ -4591,7 +4598,7 @@
         <v>150</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
         <v>2.5</v>
@@ -4630,7 +4637,7 @@
         <v>150</v>
       </c>
       <c r="D22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
         <v>2.5</v>
@@ -6871,7 +6878,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tower Ability Time and Speed
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDB3505-CBD5-4DFD-AB66-DC57EE8D67EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAB9A89-DEBD-464A-B5E6-95F6E46844B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28455" yWindow="5730" windowWidth="18075" windowHeight="14130" tabRatio="831" firstSheet="1" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-28485" yWindow="5850" windowWidth="21735" windowHeight="14130" tabRatio="831" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="TOWER@FIRE" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="247">
   <si>
     <t>ATTACKSPEED</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -943,30 +943,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>202,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>203,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>102,1;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>200,0.4;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>201,0.5;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AbilityType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1007,15 +983,46 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0,2;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,1.5;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101,1;</t>
+    <t>201,3,0,0.5;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>201,3,0,0.5;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,3,0,1.5;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,0,0,2;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>202,2.5,0,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>203,2,0,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101,5,0.3,1;</t>
+  </si>
+  <si>
+    <t>101,5,0.3,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102,5,0.3,1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200,2.5,0,0.4;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101,5,0.4,1;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1392,9 +1399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F370FB-69E7-436B-99AD-BE543F2F51A7}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1405,7 +1412,7 @@
     <col min="12" max="12" width="12" style="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
     <col min="14" max="14" width="9" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9" style="1"/>
+    <col min="15" max="15" width="22.5" style="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1"/>
     <col min="20" max="16384" width="9" style="1"/>
@@ -1496,7 +1503,7 @@
         <v>61</v>
       </c>
       <c r="O2" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="P2" s="1" t="str">
         <f t="shared" ref="P2:P23" si="0">CONCATENATE("/Sprites/Tower/",A2,"/")</f>
@@ -1544,7 +1551,7 @@
         <v>0.3</v>
       </c>
       <c r="O3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="P3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1595,7 +1602,7 @@
         <v>61</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="P4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1754,7 +1761,7 @@
         <v>0.3</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="P8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2573,9 +2580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3F0F3C-A656-4EC0-A859-21F1263F0A34}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2584,6 +2591,7 @@
     <col min="9" max="9" width="9" style="1"/>
     <col min="10" max="11" width="9" style="1" customWidth="1"/>
     <col min="12" max="13" width="9" style="1"/>
+    <col min="15" max="15" width="22.5" customWidth="1"/>
     <col min="16" max="16" width="25" style="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1"/>
     <col min="20" max="16384" width="9" style="1"/>
@@ -2671,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="P2" s="1" t="str">
         <f t="shared" ref="P2:P23" si="0">CONCATENATE("/Sprites/Tower/",A2,"/")</f>
@@ -3677,9 +3685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4F02CE-18E1-4CEC-BC57-9C41A68A4035}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
+      <selection pane="bottomLeft" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3690,7 +3698,7 @@
     <col min="10" max="11" width="9" style="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
     <col min="14" max="14" width="9" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9" style="1"/>
+    <col min="15" max="15" width="22.5" style="1" customWidth="1"/>
     <col min="16" max="16" width="25" style="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1"/>
     <col min="20" max="16384" width="9" style="1"/>
@@ -3790,7 +3798,7 @@
         <v>117</v>
       </c>
       <c r="O2" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="P2" s="1" t="str">
         <f t="shared" ref="P2:P25" si="0">CONCATENATE("/Sprites/Tower/",A2,"/")</f>
@@ -3887,7 +3895,7 @@
         <v>0.1</v>
       </c>
       <c r="O4" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="P4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4538,7 +4546,7 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="P19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4577,7 +4585,7 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="P20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4616,7 +4624,7 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="P21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4655,7 +4663,7 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="P22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -4703,7 +4711,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="O23" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="P23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -7021,34 +7029,34 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G9" t="s">
+        <v>233</v>
+      </c>
+      <c r="H9" t="s">
         <v>232</v>
       </c>
-      <c r="B9" t="s">
-        <v>233</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="I9" t="s">
         <v>234</v>
       </c>
-      <c r="D9" t="s">
+      <c r="J9" t="s">
         <v>235</v>
-      </c>
-      <c r="E9" t="s">
-        <v>236</v>
-      </c>
-      <c r="F9" t="s">
-        <v>237</v>
-      </c>
-      <c r="G9" t="s">
-        <v>239</v>
-      </c>
-      <c r="H9" t="s">
-        <v>238</v>
-      </c>
-      <c r="I9" t="s">
-        <v>240</v>
-      </c>
-      <c r="J9" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>